<commit_message>
can fetch from trello and convert into json file
</commit_message>
<xml_diff>
--- a/auth.xlsx
+++ b/auth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Trello-Google Sheet Aid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76F9EA3-50F3-425C-9962-6D60A8FC3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D43C5D-7B4E-4051-89EB-DA47B82DF02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Board Name</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>61bd066a3e19af6457869b23</t>
+  </si>
+  <si>
+    <t>Short ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3aSxVQ8E</t>
+  </si>
+  <si>
+    <t>wZlfoT6y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1DySJs3m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -109,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -391,80 +407,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.06640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>